<commit_message>
Changes to search page
Form validation with error modal popup.
Searching gif
Popup window shows the number of results.
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3E06A1F2-55F2-454B-8296-1C6249258653}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE638A6-62FD-427D-96E5-87E7473EDC95}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>login page</t>
   </si>
@@ -151,13 +151,31 @@
   </si>
   <si>
     <t>Ενέργειες</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ναι, Πρέπει να τροποποιηθεί με τεχνολογία ajax
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Δημήτρης: Τα αεροδρόμια ήδη γίνονται retrieve με ajax</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +188,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
@@ -204,7 +231,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -220,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -543,7 +570,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +578,7 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -681,7 +708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -689,8 +716,8 @@
         <v>33</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" t="s">
-        <v>35</v>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,7 +785,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Retrieving Flight Data (Not Ready 1)
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDFB7E4-8410-4704-9ED0-65451B033635}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1D28EC40-E012-408F-B8E8-9576A454E5F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>login page</t>
   </si>
@@ -258,9 +258,6 @@
     <t>5.7</t>
   </si>
   <si>
-    <t>5.8</t>
-  </si>
-  <si>
     <t>6.1</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
   </si>
   <si>
     <t>Το site μας θα είναι στα ελληνικά η english?</t>
-  </si>
-  <si>
-    <t>Ιδέες παρακαλώ…</t>
   </si>
   <si>
     <t>Τώρα είναι και τα δύο</t>
@@ -297,13 +291,22 @@
   </si>
   <si>
     <t>Υλοποιήθηκε μερικώς. Θα είναι στα αγγλικά</t>
+  </si>
+  <si>
+    <t>Ναι, υλοποιήθηκε με Jquery</t>
+  </si>
+  <si>
+    <t>Κώστας, Νάσια</t>
+  </si>
+  <si>
+    <t>Εν' αναμονή του Token</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +357,14 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -375,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -390,9 +401,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,7 +422,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -728,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +770,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1091,10 +1105,10 @@
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1116,7 +1130,7 @@
         <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>20</v>
@@ -1171,107 +1185,110 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>6</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>6</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>36</v>
+      <c r="D38" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E38">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>25</v>
+      <c r="D39" t="s">
+        <v>78</v>
       </c>
       <c r="E39">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>7</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>20</v>
+      <c r="C43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" t="s">
+        <v>73</v>
       </c>
       <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Find airline from Base
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
   <si>
     <t>login page</t>
   </si>
@@ -342,6 +342,21 @@
   </si>
   <si>
     <t>Εκκρεμεί</t>
+  </si>
+  <si>
+    <t>5.2.3</t>
+  </si>
+  <si>
+    <t>Εάν δεν βρεί το αεροδρόμιο στην ΒΔ, να το αναζητεί από το API.</t>
+  </si>
+  <si>
+    <t>5.2.4</t>
+  </si>
+  <si>
+    <t>Εάν δεν βρεί την αεροπορική εταιρία στην ΒΔ, να την αναζητεί από το API.</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
@@ -476,9 +491,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -495,6 +507,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -800,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +979,7 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E11">
@@ -981,7 +996,7 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>89</v>
       </c>
       <c r="E12">
@@ -998,7 +1013,7 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E13">
@@ -1112,7 +1127,7 @@
       <c r="C21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E21">
@@ -1129,7 +1144,7 @@
       <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E22">
@@ -1181,7 +1196,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>91</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -1249,89 +1264,89 @@
       <c r="C33" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>97</v>
+      <c r="D33" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35">
-        <v>6</v>
+      <c r="D35" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>97</v>
+        <v>69</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E38">
@@ -1339,168 +1354,202 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="4"/>
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>6</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
         <v>71</v>
       </c>
-      <c r="E43">
+      <c r="E45">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>7</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D48" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E46">
+      <c r="E48">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
+    <row r="49" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E47">
+      <c r="E49">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="12" t="s">
+      <c r="B53" s="20"/>
+      <c r="C53" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+    <row r="54" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C54" s="14">
         <v>43441</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="17">
+      <c r="C55" s="16">
         <v>43434</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="17">
+      <c r="C56" s="16">
         <v>43427</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="17">
+      <c r="C57" s="16">
         <v>43408</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A53:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Captcha in registration form and Update Todo
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\flights\Tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07C873FB-2E57-4B36-9921-33DC9FFB12E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C4DDF-11D8-4665-8BE7-49A640E0F4DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,15 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="138">
   <si>
     <t>login page</t>
   </si>
   <si>
     <t>a/a</t>
-  </si>
-  <si>
-    <t>captcha</t>
   </si>
   <si>
     <t>main page</t>
@@ -308,12 +305,6 @@
     <t>V1.2 Mobile Ready Web Application</t>
   </si>
   <si>
-    <t>Νάσια, Δημήτρης</t>
-  </si>
-  <si>
-    <t>ΕΔΩ ΔΗΜΗΤΡΗ ΤΑ ΠΡΟΗΓΟΥΜΕΝΑ ΒΗΜΑΤΑ</t>
-  </si>
-  <si>
     <t>Δημιουργία κλήσης αεροδρομίων στην ΒΔ</t>
   </si>
   <si>
@@ -465,13 +456,25 @@
   </si>
   <si>
     <t>Έγινε με Javascript/JS Object στην V2.0</t>
+  </si>
+  <si>
+    <t>captcha στην εγγραφή νέου χρήστη</t>
+  </si>
+  <si>
+    <t>Τράβηγμα δεδομένων API με Php code</t>
+  </si>
+  <si>
+    <t>Τράβηγμα των αεροδρομίων άφιξης και αναχώρησης με την php function: file_get_contents()</t>
+  </si>
+  <si>
+    <t>Τράβηγμα αποτελεσμάτων της αναζήτησης του api με την php function: file_get_contents()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,15 +525,6 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -567,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -579,9 +573,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -590,9 +581,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -605,9 +593,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -634,9 +619,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -652,7 +643,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -974,405 +965,405 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="51.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>63</v>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>81</v>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>81</v>
+      <c r="A4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>81</v>
+      <c r="A5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>81</v>
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>81</v>
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>81</v>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>90</v>
+      <c r="A11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>96</v>
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="E12" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>96</v>
+      <c r="A13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>3</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="B15" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>81</v>
+      <c r="A16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>81</v>
+      <c r="A17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>81</v>
+      <c r="C18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E18" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>81</v>
+      <c r="C19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E19" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>81</v>
+      <c r="C20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>90</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>90</v>
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>4</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="10">
+      <c r="C25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>5</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="B27" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1382,626 +1373,638 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="C32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>136</v>
       </c>
       <c r="E33" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>69</v>
+      <c r="A34" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="E34" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>69</v>
+      <c r="A35" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="E35" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>90</v>
+      <c r="A36" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="11" t="s">
+      <c r="A37" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>90</v>
+      <c r="A38" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>80</v>
+      <c r="B40" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E40" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="11" t="s">
+      <c r="A41" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="B42" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>90</v>
+      <c r="C42" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E42" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>90</v>
+      <c r="A43" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E43" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44" s="11" t="s">
+      <c r="A44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>90</v>
+      <c r="A45" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E45" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>90</v>
+      <c r="A46" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>90</v>
+      <c r="A47" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E47" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="12"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>6</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
+      <c r="B49" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>31</v>
+      <c r="A50" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="E50" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>79</v>
+      <c r="A51" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E51" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>110</v>
+      <c r="A52" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="E52" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="7"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="6"/>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>7</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
+      <c r="B54" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>90</v>
+      <c r="A55" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E55" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="11" t="s">
+      <c r="A56" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>67</v>
       </c>
       <c r="E56" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>90</v>
+      <c r="B59" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E59" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>90</v>
+      <c r="A60" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E60" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="11" t="s">
+      <c r="A61" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" s="11" t="s">
+      <c r="B64" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C64" s="11"/>
-      <c r="D64" s="13" t="s">
-        <v>90</v>
+      <c r="C64" s="9"/>
+      <c r="D64" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="7"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="6"/>
       <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="19"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="16"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="11" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C68" s="18">
+      <c r="A68" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" s="15">
         <v>43443</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C69" s="18">
+        <v>72</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="15">
         <v>43441</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="18">
+        <v>73</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="15">
         <v>43434</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="18">
+        <v>74</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="15">
         <v>43427</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="18">
+      <c r="C72" s="15">
         <v>43408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Getairport by api not working...
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A9B19A3-F495-4169-A6B7-4023AB3DD6ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D712CD9B-E65F-4EE1-945E-8699957A1868}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
   <si>
     <t>login page</t>
   </si>
@@ -326,9 +326,6 @@
     <t>5.2.4</t>
   </si>
   <si>
-    <t>Εάν δεν βρεί την αεροπορική εταιρία στην ΒΔ, να την αναζητεί από το API.</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
     <t>Ενσωμάτωση token στις κλήσεις 5.2.1, 5.2.2</t>
   </si>
   <si>
-    <t>5.2.5</t>
-  </si>
-  <si>
     <t>5.4.1</t>
   </si>
   <si>
@@ -486,6 +480,9 @@
   </si>
   <si>
     <t>V2.2</t>
+  </si>
+  <si>
+    <t>Front end Improvements</t>
   </si>
 </sst>
 </file>
@@ -637,19 +634,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -990,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,12 +1023,12 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -1095,12 +1092,12 @@
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1158,7 +1155,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>19</v>
@@ -1181,7 +1178,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" s="2">
         <v>4</v>
@@ -1198,7 +1195,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
@@ -1215,12 +1212,12 @@
       <c r="A15" s="3">
         <v>3</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -1312,7 +1309,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>18</v>
@@ -1335,7 +1332,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
@@ -1352,12 +1349,12 @@
       <c r="A24" s="3">
         <v>4</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
@@ -1368,7 +1365,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" s="8">
         <v>1</v>
@@ -1385,12 +1382,12 @@
       <c r="A27" s="3">
         <v>5</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1401,10 +1398,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>18</v>
@@ -1418,10 +1415,10 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>18</v>
@@ -1435,10 +1432,10 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>18</v>
@@ -1455,7 +1452,7 @@
         <v>51</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>18</v>
@@ -1478,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E33" s="2">
         <v>10</v>
@@ -1523,7 +1520,7 @@
         <v>87</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>18</v>
@@ -1549,93 +1546,93 @@
         <v>86</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>86</v>
       </c>
       <c r="E42" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>99</v>
       </c>
@@ -1643,38 +1640,38 @@
         <v>100</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>105</v>
+      <c r="E44" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>19</v>
@@ -1688,10 +1685,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>19</v>
@@ -1704,151 +1701,149 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="2">
-        <v>4</v>
-      </c>
+      <c r="A47" s="6"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="2"/>
+      <c r="A48" s="3">
+        <v>6</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>6</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>30</v>
+      <c r="D50" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="E50" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="E51" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" s="2">
-        <v>5</v>
-      </c>
+      <c r="A52" s="6"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+      <c r="A53" s="3">
         <v>7</v>
       </c>
-      <c r="B54" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
+      <c r="B53" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>86</v>
+        <v>64</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="E55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E56" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="D57" s="11" t="s">
         <v>86</v>
       </c>
@@ -1859,36 +1854,38 @@
         <v>112</v>
       </c>
       <c r="B58" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="B59" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>119</v>
@@ -1897,36 +1894,34 @@
         <v>17</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E60" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>138</v>
+        <v>18</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>86</v>
@@ -1935,161 +1930,150 @@
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>126</v>
-      </c>
       <c r="C63" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E63" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="9" t="s">
+      <c r="D64" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E64" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="D65" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B66" s="23" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="16"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="23"/>
+      <c r="C68" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="16"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="9" t="s">
-        <v>70</v>
+      <c r="B69" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="15">
+        <v>43449</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="9"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+      <c r="A70" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="14" t="s">
-        <v>94</v>
+      <c r="C70" s="15">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="C71" s="15">
-        <v>43443</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C72" s="15">
-        <v>43441</v>
+        <v>43434</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73" s="15">
-        <v>43434</v>
+        <v>43427</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C74" s="15">
-        <v>43427</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="15">
         <v>43408</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B48:E48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
V2.3 Forgot Password Functioning
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\flights\Tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D712CD9B-E65F-4EE1-945E-8699957A1868}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CC972C1C-E833-4BB5-9600-109AEDAD532F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="151">
   <si>
     <t>login page</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Ανάκτηση επιλογών χρήστη</t>
-  </si>
-  <si>
-    <t>Μερικώς</t>
   </si>
   <si>
     <t>Υπεύθυνος</t>
@@ -476,13 +473,40 @@
     <t>To apikey να χρησιμοποιείται sto Backend από το config.php και στο frontend από το sessionStorage('apikey')</t>
   </si>
   <si>
-    <t>Να δημιου δυνατότητα ανάκτησης password</t>
-  </si>
-  <si>
     <t>V2.2</t>
   </si>
   <si>
     <t>Front end Improvements</t>
+  </si>
+  <si>
+    <t>Δυνατότητα ανάκτησης password</t>
+  </si>
+  <si>
+    <t>Ναι στην V2.3</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>Δυνατότητα αλλαγής στοιχείων πελάτη</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
+  <si>
+    <t>Δυνατότητα αλλαγής password πελάτη</t>
+  </si>
+  <si>
+    <t>7.13</t>
+  </si>
+  <si>
+    <t>Να μπει το όνομα του χρήστη στο μενού (μόνο στις μεγάλες αναλύσεις)</t>
+  </si>
+  <si>
+    <t>V2.3</t>
+  </si>
+  <si>
+    <t>Forgot Password. Minor bugs, improvements</t>
   </si>
 </sst>
 </file>
@@ -526,7 +550,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFC000"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
@@ -534,7 +558,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
@@ -576,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -606,14 +630,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -640,14 +661,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,79 +1037,79 @@
         <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
@@ -1092,25 +1119,25 @@
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -1121,13 +1148,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
@@ -1135,16 +1162,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1152,464 +1179,460 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>86</v>
+      <c r="D11" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>9</v>
+        <v>143</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="2">
-        <v>4</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
+      <c r="B17" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="2"/>
+      <c r="A23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>4</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="A24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>4</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="8">
+      <c r="D27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>5</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>127</v>
+      <c r="B29" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>124</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>51</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E32" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>52</v>
+      <c r="A33" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="E33" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E34" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="E35" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>78</v>
+      <c r="D39" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="E39" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="C40" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>86</v>
+      <c r="D41" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="E41" s="2">
         <v>6</v>
@@ -1617,463 +1640,529 @@
     </row>
     <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="C44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="B45" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="C45" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E44" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="D45" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="2">
-        <v>4</v>
+        <v>85</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="2"/>
+      <c r="A47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+      <c r="A48" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
         <v>6</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B50" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="2">
-        <v>5</v>
-      </c>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D51" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E51" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>7</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E51" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>7</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="9" t="s">
+      <c r="B56" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D54" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="2">
+      <c r="D56" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E58" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E59" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="D59" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="C61" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>86</v>
+        <v>17</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E63" s="2">
-        <v>0.5</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>135</v>
+        <v>119</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>139</v>
+        <v>120</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="16"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="17"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="15"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="24"/>
+      <c r="C71" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="23"/>
-      <c r="C68" s="9" t="s">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="14">
+        <v>43458</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" s="14">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C74" s="14">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B69" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C69" s="15">
-        <v>43449</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C70" s="15">
-        <v>43443</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="B75" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C75" s="14">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="15">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="B76" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" s="14">
+        <v>43434</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C72" s="15">
-        <v>43434</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="B77" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="14">
+        <v>43427</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" s="15">
-        <v>43427</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="B78" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C74" s="15">
+      <c r="C78" s="14">
         <v>43408</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B50:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Popup In Flights scanner menu brand
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\flights\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{048D7747-D730-429F-B4EE-192C87113C4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C93B3182-631F-45A2-A874-5E5882CD68D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,8 +1866,8 @@
       <c r="C56" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="11" t="s">
-        <v>85</v>
+      <c r="D56" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="E56" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
V2.5 Setting Page Up and running!!!
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="160">
   <si>
     <t>login page</t>
   </si>
@@ -472,9 +472,6 @@
     <t>V2.4</t>
   </si>
   <si>
-    <t>Save, Load, Delete filters working perfectly</t>
-  </si>
-  <si>
     <t>Κώστας: Επικοινώνησα με Ουγιάρογλου, αναμενουμε. Δεν απάντησε ο Ουγιάρογλου.</t>
   </si>
   <si>
@@ -491,6 +488,18 @@
   </si>
   <si>
     <t>Μετατροπή όλων των alerts &amp; prompts σε αντίστοιχα modals</t>
+  </si>
+  <si>
+    <t>Ναι στην V2.5</t>
+  </si>
+  <si>
+    <t>V2.5</t>
+  </si>
+  <si>
+    <t>Change profile settings</t>
+  </si>
+  <si>
+    <t>Save, Load, Delete search filters</t>
   </si>
 </sst>
 </file>
@@ -583,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -658,6 +667,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -969,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,12 +1017,12 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1074,12 +1086,12 @@
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1159,10 +1171,12 @@
       <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="D12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1224,12 +1238,12 @@
       <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -1361,12 +1375,12 @@
       <c r="A26" s="3">
         <v>4</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
@@ -1394,12 +1408,12 @@
       <c r="A29" s="3">
         <v>5</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -1572,7 +1586,7 @@
         <v>97</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E40" s="2"/>
     </row>
@@ -1587,7 +1601,7 @@
         <v>18</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" s="2">
         <v>6</v>
@@ -1615,13 +1629,13 @@
         <v>95</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>97</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E43" s="2">
         <v>6</v>
@@ -1655,7 +1669,7 @@
         <v>97</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E45" s="2">
         <v>6</v>
@@ -1672,7 +1686,7 @@
         <v>19</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
@@ -1689,7 +1703,7 @@
         <v>19</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E47" s="2">
         <v>4</v>
@@ -1706,7 +1720,7 @@
         <v>19</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="2">
         <v>4</v>
@@ -1723,12 +1737,12 @@
       <c r="A50" s="3">
         <v>6</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
@@ -1792,12 +1806,12 @@
       <c r="A55" s="3">
         <v>7</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
@@ -1928,10 +1942,12 @@
       <c r="C63" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E63" s="2"/>
+      <c r="D63" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
@@ -1961,7 +1977,7 @@
         <v>117</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E65" s="2"/>
     </row>
@@ -2031,16 +2047,16 @@
     </row>
     <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="21" t="s">
         <v>155</v>
-      </c>
-      <c r="B70" s="21" t="s">
-        <v>156</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E70" s="2">
         <v>5</v>
@@ -2061,99 +2077,110 @@
       <c r="E72" s="15"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="27" t="s">
+      <c r="A73" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="27"/>
+      <c r="B73" s="28"/>
       <c r="C73" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="25" t="s">
+      <c r="A74" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="14">
+        <v>43471</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="B74" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C74" s="14">
-        <v>43469</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="22" t="s">
+      <c r="B75" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C75" s="14">
+        <v>43468</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="23" t="s">
+      <c r="B76" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="C75" s="14">
+      <c r="C76" s="14">
         <v>43461</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="B77" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C76" s="14">
+      <c r="C77" s="14">
         <v>43449</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B78" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C77" s="14">
+      <c r="C78" s="14">
         <v>43443</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="79" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C78" s="14">
+      <c r="C79" s="14">
         <v>43441</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C79" s="14">
-        <v>43434</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C80" s="14">
-        <v>43427</v>
+        <v>43434</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C81" s="14">
+        <v>43427</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B82" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C81" s="14">
+      <c r="C82" s="14">
         <v>43408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final upload... Ready for presenation!
</commit_message>
<xml_diff>
--- a/Tasks/To Do.xlsx
+++ b/Tasks/To Do.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flights\Tasks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D7F459CB-9337-4312-B3C6-2D4F75255C53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="159">
   <si>
     <t>login page</t>
   </si>
@@ -269,9 +275,6 @@
   </si>
   <si>
     <t>Δημιουργία κλήσης airliners στην ΒΔ</t>
-  </si>
-  <si>
-    <t>Εκκρεμεί</t>
   </si>
   <si>
     <t>5.2.3</t>
@@ -505,8 +508,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,14 +538,6 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="161"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
@@ -592,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -601,9 +596,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -659,13 +651,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -737,7 +726,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -770,9 +759,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,6 +811,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -980,36 +1003,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="51.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1017,24 +1040,24 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E3" s="2">
@@ -1042,16 +1065,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="2">
@@ -1059,16 +1082,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E5" s="2">
@@ -1076,34 +1099,34 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="2">
@@ -1111,16 +1134,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E9" s="2">
@@ -1128,16 +1151,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E10" s="2">
@@ -1145,117 +1168,119 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="E11" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>156</v>
+      <c r="D12" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="E12" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="2"/>
+      <c r="D13" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>87</v>
+      <c r="D14" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="E14" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>87</v>
+      <c r="D15" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="2">
@@ -1263,16 +1288,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E19" s="2">
@@ -1280,16 +1305,16 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="2">
@@ -1297,16 +1322,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E21" s="2">
@@ -1314,16 +1339,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E22" s="2">
@@ -1331,16 +1356,16 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E23" s="2">
@@ -1348,176 +1373,186 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>129</v>
+      <c r="D24" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>4</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="8">
+      <c r="D27" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>5</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="A30" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D32" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="E32" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>72</v>
+      <c r="D33" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E33" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="E34" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="9" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>122</v>
+      <c r="D35" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="E35" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="9" t="s">
+      <c r="A36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>66</v>
       </c>
       <c r="E36" s="2">
@@ -1525,675 +1560,660 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>66</v>
+      <c r="A37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="E37" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>136</v>
+      <c r="D38" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="E38" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="9" t="s">
+      <c r="A39" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="D40" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E41" s="2">
+    <row r="44" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E42" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="9" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E43" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>153</v>
-      </c>
       <c r="E45" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="9" t="s">
+      <c r="A46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>153</v>
+      <c r="D46" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="9" t="s">
+      <c r="A47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>153</v>
+      <c r="D47" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="E47" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="2">
-        <v>4</v>
-      </c>
+      <c r="A48" s="5"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="2"/>
+      <c r="A49" s="3">
+        <v>6</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>6</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A50" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>136</v>
+      <c r="D50" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E51" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>75</v>
+      <c r="D52" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="E52" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="10" t="s">
+      <c r="A53" s="5"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>7</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E53" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>7</v>
-      </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="9" t="s">
+      <c r="B57" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E57" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>136</v>
+      <c r="D58" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="E58" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" s="9" t="s">
+      <c r="A59" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="B59" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E59" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="9" t="s">
+      <c r="D62" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E61" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>156</v>
+      <c r="D63" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="E63" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="D64" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E64" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B65" s="21" t="s">
+      <c r="D65" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D65" s="26" t="s">
-        <v>150</v>
-      </c>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B66" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" s="9" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E66" s="2"/>
+      <c r="D66" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B67" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>136</v>
+      <c r="A67" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="E67" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E69" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="16"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="14"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" s="26"/>
+      <c r="C72" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="13">
+        <v>43471</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="13">
+        <v>43468</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E68" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B69" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B70" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E70" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="15"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" s="28"/>
-      <c r="C73" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="C74" s="14">
-        <v>43471</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="C75" s="14">
-        <v>43468</v>
+      <c r="B75" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" s="13">
+        <v>43461</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="B76" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="C76" s="14">
-        <v>43461</v>
+      <c r="A76" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C76" s="13">
+        <v>43449</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C77" s="14">
-        <v>43449</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+      <c r="A77" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C78" s="14">
+      <c r="C77" s="13">
         <v>43443</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" s="13">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" s="14">
-        <v>43441</v>
+        <v>70</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="13">
+        <v>43434</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C80" s="14">
-        <v>43434</v>
+        <v>71</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" s="13">
+        <v>43427</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="14">
-        <v>43427</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B81" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C82" s="14">
+      <c r="C81" s="13">
         <v>43408</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B49:E49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2204,7 +2224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2218,7 +2238,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>

</xml_diff>